<commit_message>
Adding sample upload files.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-clients-upload.xlsx
+++ b/data/_orig/pmhc-clients-upload.xlsx
@@ -1,21 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec-wayback/data/_orig/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04F67537-8B14-BE4C-8F6A-1FDB2627031F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47060" yWindow="3500" windowWidth="25360" windowHeight="15820" activeTab="2"/>
+    <workbookView xWindow="14600" yWindow="3880" windowWidth="24980" windowHeight="16660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
     <sheet name="Organisations" sheetId="8" r:id="rId2"/>
     <sheet name="Clients" sheetId="1" r:id="rId3"/>
     <sheet name="Episodes" sheetId="2" r:id="rId4"/>
-    <sheet name="NSPT Episodes" sheetId="11" r:id="rId5"/>
-    <sheet name="SIDAS" sheetId="12" r:id="rId6"/>
+    <sheet name="TWB Episodes" sheetId="11" r:id="rId5"/>
+    <sheet name="TWB PNPCs" sheetId="14" r:id="rId6"/>
+    <sheet name="TWB Critical Incidents" sheetId="15" r:id="rId7"/>
+    <sheet name="TWB Recommendation Outs" sheetId="16" r:id="rId8"/>
+    <sheet name="Collection Occasions" sheetId="18" r:id="rId9"/>
+    <sheet name="K10+" sheetId="19" r:id="rId10"/>
+    <sheet name="K5" sheetId="23" r:id="rId11"/>
+    <sheet name="SDQ" sheetId="24" r:id="rId12"/>
+    <sheet name="WHO-5" sheetId="22" r:id="rId13"/>
+    <sheet name="SIDAS" sheetId="12" r:id="rId14"/>
+    <sheet name="TWB Plans" sheetId="20" r:id="rId15"/>
+    <sheet name="TWB NIs" sheetId="21" r:id="rId16"/>
+    <sheet name="Service Contacts" sheetId="13" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="253">
   <si>
     <t>organisation_path</t>
   </si>
@@ -146,9 +171,6 @@
     <t>collection_occasion_key</t>
   </si>
   <si>
-    <t>measure_date</t>
-  </si>
-  <si>
     <t>reason_for_collection</t>
   </si>
   <si>
@@ -209,30 +231,6 @@
     <t>version</t>
   </si>
   <si>
-    <t>nspt_consent_flag</t>
-  </si>
-  <si>
-    <t>nspt_consumer_survey</t>
-  </si>
-  <si>
-    <t>nspt_sexual_identity</t>
-  </si>
-  <si>
-    <t>nspt_veteran</t>
-  </si>
-  <si>
-    <t>nspt_main_treatment_focus</t>
-  </si>
-  <si>
-    <t>nspt_other_services</t>
-  </si>
-  <si>
-    <t>nspt_lifetime_suicide_attempt</t>
-  </si>
-  <si>
-    <t>nspt_referral_made</t>
-  </si>
-  <si>
     <t>nspt_tags</t>
   </si>
   <si>
@@ -275,16 +273,61 @@
     <t>CL0002-E01</t>
   </si>
   <si>
-    <t>7 5</t>
-  </si>
-  <si>
-    <t>tag3, !nspt</t>
-  </si>
-  <si>
-    <t>!nspt</t>
-  </si>
-  <si>
-    <t>NSPT</t>
+    <t>service_contact_key</t>
+  </si>
+  <si>
+    <t>practitioner_key</t>
+  </si>
+  <si>
+    <t>service_contact_date</t>
+  </si>
+  <si>
+    <t>service_contact_type</t>
+  </si>
+  <si>
+    <t>service_contact_postcode</t>
+  </si>
+  <si>
+    <t>service_contact_modality</t>
+  </si>
+  <si>
+    <t>service_contact_participants</t>
+  </si>
+  <si>
+    <t>service_contact_venue</t>
+  </si>
+  <si>
+    <t>service_contact_duration</t>
+  </si>
+  <si>
+    <t>service_contact_copayment</t>
+  </si>
+  <si>
+    <t>service_contact_participation_indicator</t>
+  </si>
+  <si>
+    <t>service_contact_interpreter</t>
+  </si>
+  <si>
+    <t>service_contact_no_show</t>
+  </si>
+  <si>
+    <t>service_contact_final</t>
+  </si>
+  <si>
+    <t>service_contact_tags</t>
+  </si>
+  <si>
+    <t>CL0001-E01-SC01</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>CL0002-E01-SC01</t>
+  </si>
+  <si>
+    <t>P02</t>
   </si>
   <si>
     <t>organisation_start_date</t>
@@ -294,15 +337,496 @@
   </si>
   <si>
     <t>continuity_of_support</t>
+  </si>
+  <si>
+    <t>tag3, !wayback</t>
+  </si>
+  <si>
+    <t>!wayback</t>
+  </si>
+  <si>
+    <t>WAYBACK</t>
+  </si>
+  <si>
+    <t>twb_veteran</t>
+  </si>
+  <si>
+    <t>twb_sexual_orientation</t>
+  </si>
+  <si>
+    <t>twb_intersex_status</t>
+  </si>
+  <si>
+    <t>twb_eligibility_type</t>
+  </si>
+  <si>
+    <t>twb_external_evaluator_contact_consent</t>
+  </si>
+  <si>
+    <t>twb_primary_nominated_professional</t>
+  </si>
+  <si>
+    <t>twb_previous_suicide_attempts</t>
+  </si>
+  <si>
+    <t>twb_transgender_status</t>
+  </si>
+  <si>
+    <t>twb_method_of_suicide_attempt</t>
+  </si>
+  <si>
+    <t>twb_pnpc_key</t>
+  </si>
+  <si>
+    <t>PNPC04-1</t>
+  </si>
+  <si>
+    <t>PNPC05-1</t>
+  </si>
+  <si>
+    <t>twb_pnpc_reason</t>
+  </si>
+  <si>
+    <t>twb_pnpc_date</t>
+  </si>
+  <si>
+    <t>twb_pnpc_tags</t>
+  </si>
+  <si>
+    <t>twb_critical_incident_key</t>
+  </si>
+  <si>
+    <t>CI04-1</t>
+  </si>
+  <si>
+    <t>CI05-1</t>
+  </si>
+  <si>
+    <t>twb_critical_incident_type</t>
+  </si>
+  <si>
+    <t>twb_critical_incident_date</t>
+  </si>
+  <si>
+    <t>twb_critical_incident_tags</t>
+  </si>
+  <si>
+    <t>RO04-1</t>
+  </si>
+  <si>
+    <t>RO05-1</t>
+  </si>
+  <si>
+    <t>twb_recommendation_out_provider_type</t>
+  </si>
+  <si>
+    <t>twb_recommendation_out_status</t>
+  </si>
+  <si>
+    <t>twb_recommendation_out_tags</t>
+  </si>
+  <si>
+    <t>funding_source</t>
+  </si>
+  <si>
+    <t>collection_occasion_date</t>
+  </si>
+  <si>
+    <t>collection_occasion_tags</t>
+  </si>
+  <si>
+    <t>k10p_item1</t>
+  </si>
+  <si>
+    <t>k10p_item2</t>
+  </si>
+  <si>
+    <t>k10p_item3</t>
+  </si>
+  <si>
+    <t>k10p_item4</t>
+  </si>
+  <si>
+    <t>k10p_item5</t>
+  </si>
+  <si>
+    <t>k10p_item6</t>
+  </si>
+  <si>
+    <t>k10p_item7</t>
+  </si>
+  <si>
+    <t>k10p_item8</t>
+  </si>
+  <si>
+    <t>k10p_item9</t>
+  </si>
+  <si>
+    <t>k10p_item10</t>
+  </si>
+  <si>
+    <t>k10p_item11</t>
+  </si>
+  <si>
+    <t>k10p_item12</t>
+  </si>
+  <si>
+    <t>k10p_item13</t>
+  </si>
+  <si>
+    <t>k10p_item14</t>
+  </si>
+  <si>
+    <t>k10p_score</t>
+  </si>
+  <si>
+    <t>k10p_tags</t>
+  </si>
+  <si>
+    <t>measure_key</t>
+  </si>
+  <si>
+    <t>M01</t>
+  </si>
+  <si>
+    <t>M02</t>
+  </si>
+  <si>
+    <t>M03</t>
+  </si>
+  <si>
+    <t>M04</t>
+  </si>
+  <si>
+    <t>twb_plan_key</t>
+  </si>
+  <si>
+    <t>TWBP01</t>
+  </si>
+  <si>
+    <t>TWBP02</t>
+  </si>
+  <si>
+    <t>TWBP03</t>
+  </si>
+  <si>
+    <t>twb_plan_type</t>
+  </si>
+  <si>
+    <t>twb_plan_tags</t>
+  </si>
+  <si>
+    <t>twb_ni_key</t>
+  </si>
+  <si>
+    <t>TWBNI01</t>
+  </si>
+  <si>
+    <t>TWBNI02</t>
+  </si>
+  <si>
+    <t>TWBNI03</t>
+  </si>
+  <si>
+    <t>TWBNI04</t>
+  </si>
+  <si>
+    <t>twb_ni_type</t>
+  </si>
+  <si>
+    <t>twb_ni_tags</t>
+  </si>
+  <si>
+    <t>who5_item1</t>
+  </si>
+  <si>
+    <t>who5_item2</t>
+  </si>
+  <si>
+    <t>who5_item3</t>
+  </si>
+  <si>
+    <t>who5_item4</t>
+  </si>
+  <si>
+    <t>who5_item5</t>
+  </si>
+  <si>
+    <t>who5_raw_score</t>
+  </si>
+  <si>
+    <t>who5_tags</t>
+  </si>
+  <si>
+    <t>M05</t>
+  </si>
+  <si>
+    <t>M06</t>
+  </si>
+  <si>
+    <t>M07</t>
+  </si>
+  <si>
+    <t>M08</t>
+  </si>
+  <si>
+    <t>M09</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>k5_item1</t>
+  </si>
+  <si>
+    <t>k5_item2</t>
+  </si>
+  <si>
+    <t>k5_item3</t>
+  </si>
+  <si>
+    <t>k5_item4</t>
+  </si>
+  <si>
+    <t>k5_item5</t>
+  </si>
+  <si>
+    <t>k5_score</t>
+  </si>
+  <si>
+    <t>k5_tags</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>sdq_version</t>
+  </si>
+  <si>
+    <t>sdq_item1</t>
+  </si>
+  <si>
+    <t>sdq_item2</t>
+  </si>
+  <si>
+    <t>sdq_item3</t>
+  </si>
+  <si>
+    <t>sdq_item4</t>
+  </si>
+  <si>
+    <t>sdq_item5</t>
+  </si>
+  <si>
+    <t>sdq_item6</t>
+  </si>
+  <si>
+    <t>sdq_item7</t>
+  </si>
+  <si>
+    <t>sdq_item8</t>
+  </si>
+  <si>
+    <t>sdq_item9</t>
+  </si>
+  <si>
+    <t>sdq_item10</t>
+  </si>
+  <si>
+    <t>sdq_item11</t>
+  </si>
+  <si>
+    <t>sdq_item12</t>
+  </si>
+  <si>
+    <t>sdq_item13</t>
+  </si>
+  <si>
+    <t>sdq_item14</t>
+  </si>
+  <si>
+    <t>sdq_item15</t>
+  </si>
+  <si>
+    <t>sdq_item16</t>
+  </si>
+  <si>
+    <t>sdq_item17</t>
+  </si>
+  <si>
+    <t>sdq_item18</t>
+  </si>
+  <si>
+    <t>sdq_item19</t>
+  </si>
+  <si>
+    <t>sdq_item20</t>
+  </si>
+  <si>
+    <t>sdq_item21</t>
+  </si>
+  <si>
+    <t>sdq_item22</t>
+  </si>
+  <si>
+    <t>sdq_item23</t>
+  </si>
+  <si>
+    <t>sdq_item24</t>
+  </si>
+  <si>
+    <t>sdq_item25</t>
+  </si>
+  <si>
+    <t>sdq_item26</t>
+  </si>
+  <si>
+    <t>sdq_item27</t>
+  </si>
+  <si>
+    <t>sdq_item28</t>
+  </si>
+  <si>
+    <t>sdq_item29</t>
+  </si>
+  <si>
+    <t>sdq_item30</t>
+  </si>
+  <si>
+    <t>sdq_item31</t>
+  </si>
+  <si>
+    <t>sdq_item32</t>
+  </si>
+  <si>
+    <t>sdq_item33</t>
+  </si>
+  <si>
+    <t>sdq_item34</t>
+  </si>
+  <si>
+    <t>sdq_item35</t>
+  </si>
+  <si>
+    <t>sdq_item36</t>
+  </si>
+  <si>
+    <t>sdq_item37</t>
+  </si>
+  <si>
+    <t>sdq_item38</t>
+  </si>
+  <si>
+    <t>sdq_item39</t>
+  </si>
+  <si>
+    <t>sdq_item40</t>
+  </si>
+  <si>
+    <t>sdq_item41</t>
+  </si>
+  <si>
+    <t>sdq_item42</t>
+  </si>
+  <si>
+    <t>sdq_emotional_symptoms</t>
+  </si>
+  <si>
+    <t>sdq_conduct_problem</t>
+  </si>
+  <si>
+    <t>sdq_hyperactivity</t>
+  </si>
+  <si>
+    <t>sdq_peer_problem</t>
+  </si>
+  <si>
+    <t>sdq_prosocial</t>
+  </si>
+  <si>
+    <t>sdq_total</t>
+  </si>
+  <si>
+    <t>sdq_impact</t>
+  </si>
+  <si>
+    <t>sdq_tags</t>
+  </si>
+  <si>
+    <t>PC101</t>
+  </si>
+  <si>
+    <t>PC201</t>
+  </si>
+  <si>
+    <t>PY201</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>M17</t>
+  </si>
+  <si>
+    <t>twb_recommendation_out_key</t>
+  </si>
+  <si>
+    <t>TWBP04</t>
+  </si>
+  <si>
+    <t>CO06-1</t>
+  </si>
+  <si>
+    <t>CO07-1</t>
+  </si>
+  <si>
+    <t>CO08-1</t>
+  </si>
+  <si>
+    <t>CO09-1</t>
+  </si>
+  <si>
+    <t>CO10-1</t>
+  </si>
+  <si>
+    <t>CO11-1</t>
+  </si>
+  <si>
+    <t>CO12-1</t>
+  </si>
+  <si>
+    <t>CO13-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -349,24 +873,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
+    <cellStyle name="Currency 2" xfId="12" xr:uid="{615BF2FF-9DFF-5A48-82C2-A2AAEE02B1C5}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -378,9 +905,18 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="11" xr:uid="{DD9A69FF-BC7C-0C41-9B1C-A10D7F749F3F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -668,37 +1204,1822 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FC7602-69F9-924D-ACB2-1F7AE9DDB0B6}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" t="s">
+        <v>139</v>
+      </c>
+      <c r="P1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>141</v>
+      </c>
+      <c r="R1" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
+      <c r="R2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E577369-DFD1-AF46-9F7B-FAC3BDFD3973}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F457D231-E140-D747-B6C3-BCBC2C07364C}">
+  <dimension ref="A1:BB4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:BB4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T1" t="s">
+        <v>202</v>
+      </c>
+      <c r="U1" t="s">
+        <v>203</v>
+      </c>
+      <c r="V1" t="s">
+        <v>204</v>
+      </c>
+      <c r="W1" t="s">
+        <v>205</v>
+      </c>
+      <c r="X1" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>2</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>2</v>
+      </c>
+      <c r="AL2">
+        <v>8</v>
+      </c>
+      <c r="AM2">
+        <v>8</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>2</v>
+      </c>
+      <c r="AP2">
+        <v>2</v>
+      </c>
+      <c r="AQ2">
+        <v>8</v>
+      </c>
+      <c r="AR2">
+        <v>8</v>
+      </c>
+      <c r="AS2">
+        <v>8</v>
+      </c>
+      <c r="AT2">
+        <v>8</v>
+      </c>
+      <c r="AU2">
+        <v>99</v>
+      </c>
+      <c r="AV2">
+        <v>99</v>
+      </c>
+      <c r="AW2">
+        <v>99</v>
+      </c>
+      <c r="AX2">
+        <v>99</v>
+      </c>
+      <c r="AY2">
+        <v>99</v>
+      </c>
+      <c r="AZ2">
+        <v>99</v>
+      </c>
+      <c r="BA2">
+        <v>99</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>9</v>
+      </c>
+      <c r="Q3">
+        <v>9</v>
+      </c>
+      <c r="R3">
+        <v>9</v>
+      </c>
+      <c r="S3">
+        <v>9</v>
+      </c>
+      <c r="T3">
+        <v>9</v>
+      </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
+      <c r="V3">
+        <v>9</v>
+      </c>
+      <c r="W3">
+        <v>9</v>
+      </c>
+      <c r="X3">
+        <v>9</v>
+      </c>
+      <c r="Y3">
+        <v>9</v>
+      </c>
+      <c r="Z3">
+        <v>9</v>
+      </c>
+      <c r="AA3">
+        <v>9</v>
+      </c>
+      <c r="AB3">
+        <v>9</v>
+      </c>
+      <c r="AC3">
+        <v>9</v>
+      </c>
+      <c r="AD3">
+        <v>9</v>
+      </c>
+      <c r="AE3">
+        <v>8</v>
+      </c>
+      <c r="AF3">
+        <v>9</v>
+      </c>
+      <c r="AG3">
+        <v>9</v>
+      </c>
+      <c r="AH3">
+        <v>9</v>
+      </c>
+      <c r="AI3">
+        <v>9</v>
+      </c>
+      <c r="AJ3">
+        <v>9</v>
+      </c>
+      <c r="AK3">
+        <v>9</v>
+      </c>
+      <c r="AL3">
+        <v>9</v>
+      </c>
+      <c r="AM3">
+        <v>9</v>
+      </c>
+      <c r="AN3">
+        <v>8</v>
+      </c>
+      <c r="AO3">
+        <v>8</v>
+      </c>
+      <c r="AP3">
+        <v>8</v>
+      </c>
+      <c r="AQ3">
+        <v>8</v>
+      </c>
+      <c r="AR3">
+        <v>8</v>
+      </c>
+      <c r="AS3">
+        <v>8</v>
+      </c>
+      <c r="AT3">
+        <v>8</v>
+      </c>
+      <c r="AU3">
+        <v>3</v>
+      </c>
+      <c r="AV3">
+        <v>3</v>
+      </c>
+      <c r="AW3">
+        <v>6</v>
+      </c>
+      <c r="AX3">
+        <v>3</v>
+      </c>
+      <c r="AY3">
+        <v>8</v>
+      </c>
+      <c r="AZ3">
+        <v>15</v>
+      </c>
+      <c r="BA3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>8</v>
+      </c>
+      <c r="AF4">
+        <v>8</v>
+      </c>
+      <c r="AG4">
+        <v>8</v>
+      </c>
+      <c r="AH4">
+        <v>8</v>
+      </c>
+      <c r="AI4">
+        <v>8</v>
+      </c>
+      <c r="AJ4">
+        <v>8</v>
+      </c>
+      <c r="AK4">
+        <v>8</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>8</v>
+      </c>
+      <c r="AO4">
+        <v>8</v>
+      </c>
+      <c r="AP4">
+        <v>8</v>
+      </c>
+      <c r="AQ4">
+        <v>8</v>
+      </c>
+      <c r="AR4">
+        <v>8</v>
+      </c>
+      <c r="AS4">
+        <v>8</v>
+      </c>
+      <c r="AT4">
+        <v>8</v>
+      </c>
+      <c r="AU4">
+        <v>99</v>
+      </c>
+      <c r="AV4">
+        <v>99</v>
+      </c>
+      <c r="AW4">
+        <v>99</v>
+      </c>
+      <c r="AX4">
+        <v>99</v>
+      </c>
+      <c r="AY4">
+        <v>99</v>
+      </c>
+      <c r="AZ4">
+        <v>99</v>
+      </c>
+      <c r="BA4">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C46AF6-9858-EA42-8C3A-944EA1D37E5A}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3937DF6B-F596-2F48-A394-BEC04954911A}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD261D8-A18E-D348-812B-635558C877D8}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.1640625" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1"/>
+    <col min="16" max="17" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="P1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2">
+        <v>21052016</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>9999</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>7</v>
+      </c>
+      <c r="R2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3">
+        <v>15062016</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>9999</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -712,14 +3033,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
@@ -729,47 +3050,47 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
       </c>
       <c r="E2">
         <v>42543098901</v>
@@ -788,15 +3109,15 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E3">
         <v>42543098901</v>
@@ -827,19 +3148,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -874,15 +3195,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
       </c>
       <c r="D2">
         <v>17021983</v>
@@ -909,15 +3230,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
       </c>
       <c r="D3">
         <v>24092007</v>
@@ -941,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -955,20 +3276,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1:AC3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1051,21 +3375,21 @@
         <v>36</v>
       </c>
       <c r="AB1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="AC1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>18062016</v>
@@ -1143,18 +3467,18 @@
         <v>2</v>
       </c>
       <c r="AC2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>17072016</v>
@@ -1232,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1246,20 +3570,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="A1:XFD3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="11" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1267,39 +3598,42 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="K1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>107</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1314,30 +3648,33 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>83</v>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1346,18 +3683,21 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1372,59 +3712,280 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B16A333-7249-F74D-A01D-D86B3BB58BE6}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10032020</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>16032020</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CD07C4-5B66-DA47-BD85-B648E9F24605}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10032020</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>16032020</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1238216A-CB04-C54D-98D5-8C357BC0DAC5}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D673CA-7AAB-3849-A897-7F1D925D9093}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
       <c r="F1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
       </c>
       <c r="D2">
         <v>10062016</v>
@@ -1432,34 +3993,19 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>16062016</v>
@@ -1467,31 +4013,171 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-      <c r="I3">
-        <v>9</v>
-      </c>
-      <c r="J3">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <v>16062018</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>16062019</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6">
+        <v>16062016</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>16062018</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8">
+        <v>20062016</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9">
+        <v>16062016</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10">
+        <v>16062016</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11">
+        <v>16062016</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>